<commit_message>
Current owner search pack Added
</commit_message>
<xml_diff>
--- a/Input/Cook_county.xlsx
+++ b/Input/Cook_county.xlsx
@@ -19,7 +19,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -76,26 +76,13 @@
       <sz val="10"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -176,21 +163,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -199,13 +186,13 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -224,7 +211,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="1" hidden="1"/>
     </xf>
@@ -232,87 +219,78 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="1" hidden="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="1" hidden="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="1" hidden="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="2" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="1" hidden="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="1" hidden="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
       <protection locked="1" hidden="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="1" hidden="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-      <protection locked="1" hidden="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="1" hidden="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="1" hidden="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="1" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="1" hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -686,7 +664,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -700,8 +678,8 @@
     <col width="17.6328125" customWidth="1" style="6" min="7" max="7"/>
     <col width="24.36328125" customWidth="1" style="6" min="8" max="8"/>
     <col width="18" customWidth="1" style="6" min="9" max="9"/>
-    <col width="8.7265625" customWidth="1" style="6" min="10" max="57"/>
-    <col width="8.7265625" customWidth="1" style="6" min="58" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="6" min="10" max="87"/>
+    <col width="8.7265625" customWidth="1" style="6" min="88" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -717,7 +695,7 @@
       </c>
       <c r="C1" s="10" t="inlineStr">
         <is>
-          <t>Borrower Name</t>
+          <t>NAME</t>
         </is>
       </c>
       <c r="D1" s="4" t="inlineStr">
@@ -752,25 +730,29 @@
       </c>
     </row>
     <row r="2" ht="18.5" customHeight="1">
-      <c r="A2" s="32" t="inlineStr">
-        <is>
-          <t>4738472-3</t>
-        </is>
-      </c>
-      <c r="B2" s="33" t="n"/>
-      <c r="C2" s="32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">JESUS SOLIS </t>
-        </is>
-      </c>
-      <c r="D2" s="32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1620 55TH ST NW, ALBUQUERQUE, NM </t>
-        </is>
-      </c>
-      <c r="E2" s="34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> BERNALILLO</t>
+      <c r="A2" s="14" t="inlineStr">
+        <is>
+          <t>1163573-9</t>
+        </is>
+      </c>
+      <c r="B2" s="18" t="inlineStr">
+        <is>
+          <t>05-33-113-009-0000</t>
+        </is>
+      </c>
+      <c r="C2" s="36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  OBrien  Mills</t>
+        </is>
+      </c>
+      <c r="D2" s="14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  1915  Washington  Ave IL COOK  60091  County:  Cook</t>
+        </is>
+      </c>
+      <c r="E2" s="28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Cook</t>
         </is>
       </c>
       <c r="F2" s="16" t="n"/>
@@ -779,25 +761,29 @@
       <c r="I2" s="7" t="n"/>
     </row>
     <row r="3" ht="18.5" customHeight="1">
-      <c r="A3" s="32" t="inlineStr">
-        <is>
-          <t>4764926-2</t>
-        </is>
-      </c>
-      <c r="B3" s="35" t="n"/>
-      <c r="C3" s="32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LUIS MATA HERRERA </t>
-        </is>
-      </c>
-      <c r="D3" s="36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 8011 SAN JUAN RD NE, Albuquerque, </t>
-        </is>
-      </c>
-      <c r="E3" s="34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> BERNALILLO</t>
+      <c r="A3" s="14" t="inlineStr">
+        <is>
+          <t>4911805-51</t>
+        </is>
+      </c>
+      <c r="B3" s="19" t="inlineStr">
+        <is>
+          <t>03-04-300-028-1294</t>
+        </is>
+      </c>
+      <c r="C3" s="37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Jason  Henry</t>
+        </is>
+      </c>
+      <c r="D3" s="15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  11 OAK  CREEK  DR, BUFFALO  </t>
+        </is>
+      </c>
+      <c r="E3" s="28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Cook</t>
         </is>
       </c>
       <c r="F3" s="16" t="n"/>
@@ -806,25 +792,29 @@
       <c r="I3" s="7" t="n"/>
     </row>
     <row r="4" ht="18.5" customHeight="1">
-      <c r="A4" s="37" t="inlineStr">
-        <is>
-          <t>4911805-51</t>
-        </is>
-      </c>
-      <c r="B4" s="38" t="n"/>
+      <c r="A4" s="30" t="inlineStr">
+        <is>
+          <t>2366573-9</t>
+        </is>
+      </c>
+      <c r="B4" s="31" t="inlineStr">
+        <is>
+          <t>20-14-202-076-1279</t>
+        </is>
+      </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">BOBBY BANKRUPT </t>
-        </is>
-      </c>
-      <c r="D4" s="36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 11 CORELOGIC DR., NEW YORK, NY </t>
+          <t xml:space="preserve">  William  smith</t>
+        </is>
+      </c>
+      <c r="D4" s="29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  400 E 55TH  ST, CHICAGO  County:  Cook</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> New York</t>
+          <t xml:space="preserve">  Cook</t>
         </is>
       </c>
       <c r="F4" s="1" t="n"/>
@@ -833,25 +823,25 @@
       <c r="I4" s="7" t="n"/>
     </row>
     <row r="5" ht="15.5" customHeight="1">
-      <c r="A5" s="39" t="inlineStr">
-        <is>
-          <t>6256642-2</t>
+      <c r="A5" s="32" t="inlineStr">
+        <is>
+          <t>4738472-3</t>
         </is>
       </c>
       <c r="B5" s="20" t="n"/>
-      <c r="C5" s="40" t="inlineStr">
-        <is>
-          <t>GEORGE COBB</t>
+      <c r="C5" s="33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JESUS SOLIS </t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 4665 NEELY ST, CEDAR BLUFF, AL </t>
+          <t xml:space="preserve"> 1620 55TH ST NW, ALBUQUERQUE, NM </t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CHEROKEE</t>
+          <t xml:space="preserve"> BERNALILLO</t>
         </is>
       </c>
       <c r="F5" s="8" t="n"/>
@@ -860,29 +850,25 @@
       <c r="I5" s="8" t="n"/>
     </row>
     <row r="6" ht="15.5" customHeight="1">
-      <c r="A6" s="41" t="inlineStr">
-        <is>
-          <t>6410980-1</t>
-        </is>
-      </c>
-      <c r="B6" s="20" t="inlineStr">
-        <is>
-          <t>00028-0000-00004</t>
-        </is>
-      </c>
-      <c r="C6" s="42" t="inlineStr">
-        <is>
-          <t>RUSSELL ZILINSKI</t>
+      <c r="A6" s="34" t="inlineStr">
+        <is>
+          <t>4764926-2</t>
+        </is>
+      </c>
+      <c r="B6" s="20" t="n"/>
+      <c r="C6" s="35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LUIS MATA HERRERA </t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 17 MANOR RD, COLTS NECK, NJ 07722</t>
+          <t xml:space="preserve"> 8011 SAN JUAN RD NE, Albuquerque, </t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Monmouth</t>
+          <t xml:space="preserve"> BERNALILLO</t>
         </is>
       </c>
       <c r="F6" s="2" t="n"/>
@@ -891,55 +877,107 @@
       <c r="I6" s="8" t="n"/>
     </row>
     <row r="7" ht="15.5" customHeight="1">
-      <c r="A7" s="30" t="n"/>
-      <c r="B7" s="24" t="n"/>
-      <c r="C7" s="30" t="n"/>
-      <c r="D7" s="30" t="n"/>
-      <c r="E7" s="30" t="n"/>
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>4911805-51</t>
+        </is>
+      </c>
+      <c r="B7" s="20" t="n"/>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BOBBY BANKRUPT </t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11 CORELOGIC DR., NEW YORK, NY </t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> New York</t>
+        </is>
+      </c>
       <c r="F7" s="2" t="n"/>
       <c r="G7" s="8" t="n"/>
       <c r="H7" s="8" t="n"/>
       <c r="I7" s="8" t="n"/>
     </row>
     <row r="8" ht="15.5" customHeight="1">
-      <c r="A8" s="30" t="n"/>
-      <c r="B8" s="24" t="n"/>
-      <c r="C8" s="27" t="n"/>
-      <c r="D8" s="30" t="n"/>
-      <c r="E8" s="30" t="n"/>
+      <c r="A8" s="11" t="inlineStr">
+        <is>
+          <t>6256642-2</t>
+        </is>
+      </c>
+      <c r="B8" s="18" t="n"/>
+      <c r="C8" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GEORGE COBB </t>
+        </is>
+      </c>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4665 NEELY ST, CEDAR BLUFF, AL </t>
+        </is>
+      </c>
+      <c r="E8" s="28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> CHEROKEE</t>
+        </is>
+      </c>
       <c r="F8" s="2" t="n"/>
       <c r="G8" s="8" t="n"/>
       <c r="H8" s="8" t="n"/>
       <c r="I8" s="8" t="n"/>
     </row>
     <row r="9" ht="15.5" customHeight="1">
-      <c r="A9" s="31" t="n"/>
-      <c r="B9" s="24" t="n"/>
-      <c r="C9" s="29" t="n"/>
-      <c r="D9" s="23" t="n"/>
-      <c r="E9" s="23" t="n"/>
+      <c r="A9" s="11" t="inlineStr">
+        <is>
+          <t>6410980-1</t>
+        </is>
+      </c>
+      <c r="B9" s="38" t="inlineStr">
+        <is>
+          <t>00028-0000-00004</t>
+        </is>
+      </c>
+      <c r="C9" s="39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RUSSELL ZILINSKI </t>
+        </is>
+      </c>
+      <c r="D9" s="40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17 MANOR RD, COLTS NECK, NJ 07722</t>
+        </is>
+      </c>
+      <c r="E9" s="28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Monmouth</t>
+        </is>
+      </c>
       <c r="F9" s="1" t="n"/>
       <c r="G9" s="7" t="n"/>
       <c r="H9" s="7" t="n"/>
       <c r="I9" s="7" t="n"/>
     </row>
     <row r="10" ht="15.5" customHeight="1">
-      <c r="A10" s="23" t="n"/>
-      <c r="B10" s="24" t="n"/>
-      <c r="C10" s="23" t="n"/>
-      <c r="D10" s="23" t="n"/>
-      <c r="E10" s="23" t="n"/>
+      <c r="A10" s="11" t="n"/>
+      <c r="B10" s="18" t="n"/>
+      <c r="C10" s="12" t="n"/>
+      <c r="D10" s="14" t="n"/>
+      <c r="E10" s="28" t="n"/>
       <c r="F10" s="1" t="n"/>
       <c r="G10" s="7" t="n"/>
       <c r="H10" s="7" t="n"/>
       <c r="I10" s="7" t="n"/>
     </row>
     <row r="11" ht="15.5" customHeight="1">
-      <c r="A11" s="23" t="n"/>
-      <c r="B11" s="24" t="n"/>
-      <c r="C11" s="23" t="n"/>
-      <c r="D11" s="23" t="n"/>
-      <c r="E11" s="23" t="n"/>
+      <c r="A11" s="11" t="n"/>
+      <c r="B11" s="19" t="n"/>
+      <c r="C11" s="13" t="n"/>
+      <c r="D11" s="15" t="n"/>
+      <c r="E11" s="28" t="n"/>
       <c r="F11" s="1" t="n"/>
       <c r="G11" s="7" t="n"/>
       <c r="H11" s="7" t="n"/>
@@ -968,11 +1006,11 @@
       <c r="I13" s="7" t="n"/>
     </row>
     <row r="14" ht="15.5" customHeight="1">
-      <c r="A14" s="28" t="n"/>
+      <c r="A14" s="27" t="n"/>
       <c r="B14" s="24" t="n"/>
       <c r="C14" s="26" t="n"/>
-      <c r="D14" s="28" t="n"/>
-      <c r="E14" s="28" t="n"/>
+      <c r="D14" s="27" t="n"/>
+      <c r="E14" s="27" t="n"/>
       <c r="F14" s="7" t="n"/>
       <c r="G14" s="7" t="n"/>
       <c r="H14" s="7" t="n"/>
@@ -1184,7 +1222,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E2"/>
+      <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -1208,7 +1246,7 @@
           <t>1915 Washington Ave IL COOK 60091</t>
         </is>
       </c>
-      <c r="E1" s="34" t="inlineStr">
+      <c r="E1" s="28" t="inlineStr">
         <is>
           <t>COS</t>
         </is>
@@ -1233,7 +1271,7 @@
           <t>11 OAK CREEK DR, BUFFALO GROVE</t>
         </is>
       </c>
-      <c r="E2" s="34" t="inlineStr">
+      <c r="E2" s="28" t="inlineStr">
         <is>
           <t>COS</t>
         </is>

</xml_diff>

<commit_message>
committing the final changes
</commit_message>
<xml_diff>
--- a/Input/Cook_county.xlsx
+++ b/Input/Cook_county.xlsx
@@ -16,9 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="mm:ss.0;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -125,9 +126,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -162,9 +160,6 @@
     <xf numFmtId="45" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="45" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -175,6 +170,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -545,10 +546,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -560,422 +561,570 @@
     <col width="21.140625" customWidth="1" style="2" min="5" max="5"/>
     <col width="30.140625" customWidth="1" style="2" min="6" max="6"/>
     <col width="32.5703125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="14.7109375" customWidth="1" style="2" min="8" max="8"/>
+    <col width="33" customWidth="1" style="2" min="8" max="8"/>
     <col width="19.5703125" customWidth="1" style="2" min="9" max="9"/>
-    <col width="8.7109375" customWidth="1" style="2" min="10" max="31"/>
-    <col width="8.7109375" customWidth="1" style="2" min="32" max="16384"/>
+    <col width="24.140625" customWidth="1" style="2" min="10" max="10"/>
+    <col width="24.5703125" customWidth="1" style="2" min="11" max="11"/>
+    <col width="8.7109375" customWidth="1" style="2" min="12" max="32"/>
+    <col width="8.7109375" customWidth="1" style="2" min="33" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Order No</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>APN</t>
         </is>
       </c>
-      <c r="C1" s="9" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>Property Address</t>
         </is>
       </c>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="D1" s="8" t="inlineStr">
         <is>
           <t>NAME</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>City</t>
         </is>
       </c>
-      <c r="F1" s="6" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>State</t>
         </is>
       </c>
-      <c r="G1" s="8" t="inlineStr">
+      <c r="G1" s="7" t="inlineStr">
         <is>
           <t>County Name</t>
         </is>
       </c>
-      <c r="H1" s="8" t="inlineStr">
+      <c r="H1" s="7" t="inlineStr">
         <is>
           <t>GTD</t>
         </is>
       </c>
-      <c r="I1" s="17" t="inlineStr">
+      <c r="I1" s="15" t="inlineStr">
         <is>
           <t>Second Name</t>
         </is>
       </c>
-    </row>
-    <row r="2" ht="11.45" customHeight="1" s="7">
-      <c r="A2" s="10" t="n">
-        <v>1174604</v>
+      <c r="J1" s="15" t="inlineStr">
+        <is>
+          <t>Start_time</t>
+        </is>
+      </c>
+      <c r="K1" s="15" t="inlineStr">
+        <is>
+          <t>End_time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="11.45" customHeight="1" s="6">
+      <c r="A2" s="9" t="n">
+        <v>1102293</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10-31-413-002-0000</t>
-        </is>
-      </c>
-      <c r="C2" s="18" t="inlineStr">
-        <is>
-          <t>6735 W Schreiber Ave</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Todd R Strother </t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
+          <t>29-27-407-037-0000</t>
+        </is>
+      </c>
+      <c r="C2" s="16" t="inlineStr">
+        <is>
+          <t>67 Indianwood Dr</t>
+        </is>
+      </c>
+      <c r="D2" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NICOLE FISHER </t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>Thornton</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>IL- 60476</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>Cook</t>
+        </is>
+      </c>
+      <c r="H2" s="14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Documents Indexed Through: 05-05-2023 </t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="n"/>
+      <c r="J2" s="19" t="n">
+        <v>45065.64565603009</v>
+      </c>
+      <c r="K2" s="20" t="n">
+        <v>45065.64983034723</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="n">
+        <v>1091017</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>APN not Found</t>
+        </is>
+      </c>
+      <c r="C3" s="16" t="inlineStr">
+        <is>
+          <t>9249 145th St</t>
+        </is>
+      </c>
+      <c r="D3" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JONATHAN KITS </t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>Orland Park</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>IL-60462</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>Cook</t>
+        </is>
+      </c>
+      <c r="H3" s="14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Documents Indexed Through: 05-05-2023 </t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="n"/>
+      <c r="J3" s="20" t="n">
+        <v>45065.64983071759</v>
+      </c>
+      <c r="K3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="n">
+        <v>1192237</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>13-26-109-007-0000</t>
+        </is>
+      </c>
+      <c r="C4" s="16" t="inlineStr">
+        <is>
+          <t>3087 N  Haussen Ct</t>
+        </is>
+      </c>
+      <c r="D4" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Robert L Jacob </t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>Chicago</t>
         </is>
       </c>
-      <c r="F2" s="11" t="inlineStr">
-        <is>
-          <t>IL- 60631</t>
-        </is>
-      </c>
-      <c r="G2" s="4" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IL-60618 </t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
         <is>
           <t>Cook</t>
         </is>
       </c>
-      <c r="H2" s="15" t="inlineStr">
+      <c r="H4" s="14" t="inlineStr">
         <is>
           <t xml:space="preserve">Documents Indexed Through: 05-05-2023 </t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>CLAUDIA  NICHOLAS</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="F3" s="11" t="n"/>
-      <c r="G3" s="4" t="n"/>
-      <c r="H3" s="15" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="n"/>
-      <c r="C4" s="19" t="n"/>
-      <c r="D4" s="3" t="n"/>
-      <c r="E4" s="20" t="n"/>
-      <c r="F4" s="4" t="n"/>
-      <c r="G4" s="4" t="n"/>
-      <c r="H4" s="15" t="n"/>
-      <c r="I4" s="4" t="n"/>
+      <c r="I4" s="3" t="n"/>
+      <c r="J4" s="20" t="n">
+        <v>45065.6502062037</v>
+      </c>
+      <c r="K4" s="3" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="n"/>
-      <c r="B5" s="4" t="n"/>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="3" t="n"/>
-      <c r="E5" s="4" t="n"/>
-      <c r="F5" s="4" t="n"/>
-      <c r="G5" s="4" t="n"/>
-      <c r="H5" s="15" t="n"/>
-      <c r="I5" s="4" t="n"/>
+      <c r="A5" s="3" t="n"/>
+      <c r="B5" s="3" t="n"/>
+      <c r="C5" s="19" t="n"/>
+      <c r="D5" s="19" t="n"/>
+      <c r="E5" s="3" t="n"/>
+      <c r="F5" s="3" t="n"/>
+      <c r="G5" s="18" t="n"/>
+      <c r="H5" s="14" t="n"/>
+      <c r="I5" s="3" t="n"/>
+      <c r="J5" s="3" t="n"/>
+      <c r="K5" s="3" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="n"/>
-      <c r="B6" s="4" t="n"/>
-      <c r="C6" s="3" t="n"/>
-      <c r="D6" s="3" t="n"/>
-      <c r="E6" s="4" t="n"/>
-      <c r="F6" s="4" t="n"/>
-      <c r="G6" s="4" t="n"/>
-      <c r="H6" s="15" t="n"/>
-      <c r="I6" s="4" t="n"/>
+      <c r="A6" s="4" t="n"/>
+      <c r="B6" s="3" t="n"/>
+      <c r="C6" s="19" t="n"/>
+      <c r="D6" s="19" t="n"/>
+      <c r="E6" s="3" t="n"/>
+      <c r="F6" s="3" t="n"/>
+      <c r="G6" s="3" t="n"/>
+      <c r="H6" s="14" t="n"/>
+      <c r="I6" s="3" t="n"/>
+      <c r="J6" s="3" t="n"/>
+      <c r="K6" s="3" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="n"/>
-      <c r="B7" s="4" t="n"/>
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="3" t="n"/>
-      <c r="E7" s="4" t="n"/>
-      <c r="F7" s="4" t="n"/>
-      <c r="G7" s="4" t="n"/>
-      <c r="H7" s="15" t="n"/>
-      <c r="I7" s="4" t="n"/>
+      <c r="A7" s="3" t="n"/>
+      <c r="B7" s="3" t="n"/>
+      <c r="C7" s="19" t="n"/>
+      <c r="D7" s="19" t="n"/>
+      <c r="E7" s="3" t="n"/>
+      <c r="F7" s="3" t="n"/>
+      <c r="G7" s="3" t="n"/>
+      <c r="H7" s="14" t="n"/>
+      <c r="I7" s="3" t="n"/>
+      <c r="J7" s="3" t="n"/>
+      <c r="K7" s="3" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="n"/>
-      <c r="B8" s="4" t="n"/>
-      <c r="C8" s="3" t="n"/>
-      <c r="D8" s="3" t="n"/>
-      <c r="E8" s="4" t="n"/>
-      <c r="F8" s="4" t="n"/>
-      <c r="G8" s="4" t="n"/>
-      <c r="H8" s="15" t="n"/>
-      <c r="I8" s="4" t="n"/>
+      <c r="A8" s="3" t="n"/>
+      <c r="B8" s="3" t="n"/>
+      <c r="C8" s="19" t="n"/>
+      <c r="D8" s="19" t="n"/>
+      <c r="E8" s="3" t="n"/>
+      <c r="F8" s="3" t="n"/>
+      <c r="G8" s="3" t="n"/>
+      <c r="H8" s="14" t="n"/>
+      <c r="I8" s="3" t="n"/>
+      <c r="J8" s="3" t="n"/>
+      <c r="K8" s="3" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="n"/>
-      <c r="B9" s="4" t="n"/>
-      <c r="C9" s="3" t="n"/>
-      <c r="D9" s="3" t="n"/>
-      <c r="E9" s="4" t="n"/>
-      <c r="F9" s="4" t="n"/>
-      <c r="G9" s="4" t="n"/>
-      <c r="H9" s="15" t="n"/>
-      <c r="I9" s="4" t="n"/>
+      <c r="A9" s="4" t="n"/>
+      <c r="B9" s="3" t="n"/>
+      <c r="C9" s="19" t="n"/>
+      <c r="D9" s="19" t="n"/>
+      <c r="E9" s="3" t="n"/>
+      <c r="F9" s="3" t="n"/>
+      <c r="G9" s="3" t="n"/>
+      <c r="H9" s="14" t="n"/>
+      <c r="I9" s="3" t="n"/>
+      <c r="J9" s="3" t="n"/>
+      <c r="K9" s="3" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="n"/>
-      <c r="B10" s="4" t="n"/>
-      <c r="C10" s="3" t="n"/>
-      <c r="D10" s="3" t="n"/>
-      <c r="E10" s="4" t="n"/>
-      <c r="F10" s="4" t="n"/>
-      <c r="G10" s="4" t="n"/>
-      <c r="H10" s="15" t="n"/>
-      <c r="I10" s="4" t="n"/>
+      <c r="A10" s="3" t="n"/>
+      <c r="B10" s="3" t="n"/>
+      <c r="C10" s="19" t="n"/>
+      <c r="D10" s="19" t="n"/>
+      <c r="E10" s="3" t="n"/>
+      <c r="F10" s="3" t="n"/>
+      <c r="G10" s="3" t="n"/>
+      <c r="H10" s="14" t="n"/>
+      <c r="I10" s="3" t="n"/>
+      <c r="J10" s="3" t="n"/>
+      <c r="K10" s="3" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="n"/>
-      <c r="B11" s="4" t="n"/>
-      <c r="C11" s="3" t="n"/>
-      <c r="D11" s="3" t="n"/>
-      <c r="E11" s="4" t="n"/>
-      <c r="F11" s="4" t="n"/>
-      <c r="G11" s="4" t="n"/>
-      <c r="H11" s="15" t="n"/>
-      <c r="I11" s="4" t="n"/>
+      <c r="A11" s="3" t="n"/>
+      <c r="B11" s="3" t="n"/>
+      <c r="C11" s="19" t="n"/>
+      <c r="D11" s="19" t="n"/>
+      <c r="E11" s="3" t="n"/>
+      <c r="F11" s="3" t="n"/>
+      <c r="G11" s="3" t="n"/>
+      <c r="H11" s="14" t="n"/>
+      <c r="I11" s="3" t="n"/>
+      <c r="J11" s="3" t="n"/>
+      <c r="K11" s="3" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="n"/>
-      <c r="B12" s="4" t="n"/>
-      <c r="C12" s="13" t="n"/>
-      <c r="D12" s="3" t="n"/>
-      <c r="E12" s="4" t="n"/>
-      <c r="F12" s="4" t="n"/>
-      <c r="G12" s="4" t="n"/>
-      <c r="H12" s="15" t="n"/>
-      <c r="I12" s="4" t="n"/>
+      <c r="A12" s="3" t="n"/>
+      <c r="B12" s="3" t="n"/>
+      <c r="C12" s="12" t="n"/>
+      <c r="D12" s="19" t="n"/>
+      <c r="E12" s="3" t="n"/>
+      <c r="F12" s="3" t="n"/>
+      <c r="G12" s="3" t="n"/>
+      <c r="H12" s="14" t="n"/>
+      <c r="I12" s="3" t="n"/>
+      <c r="J12" s="3" t="n"/>
+      <c r="K12" s="3" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="n"/>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="13" t="n"/>
-      <c r="D13" s="3" t="n"/>
-      <c r="E13" s="4" t="n"/>
-      <c r="F13" s="4" t="n"/>
-      <c r="G13" s="4" t="n"/>
-      <c r="H13" s="15" t="n"/>
-      <c r="I13" s="4" t="n"/>
+      <c r="A13" s="3" t="n"/>
+      <c r="B13" s="4" t="n"/>
+      <c r="C13" s="12" t="n"/>
+      <c r="D13" s="19" t="n"/>
+      <c r="E13" s="3" t="n"/>
+      <c r="F13" s="3" t="n"/>
+      <c r="G13" s="3" t="n"/>
+      <c r="H13" s="14" t="n"/>
+      <c r="I13" s="3" t="n"/>
+      <c r="J13" s="3" t="n"/>
+      <c r="K13" s="3" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="n"/>
-      <c r="B14" s="4" t="n"/>
-      <c r="C14" s="13" t="n"/>
-      <c r="D14" s="3" t="n"/>
-      <c r="E14" s="4" t="n"/>
-      <c r="F14" s="4" t="n"/>
-      <c r="G14" s="4" t="n"/>
-      <c r="H14" s="15" t="n"/>
-      <c r="I14" s="4" t="n"/>
+      <c r="A14" s="3" t="n"/>
+      <c r="B14" s="3" t="n"/>
+      <c r="C14" s="12" t="n"/>
+      <c r="D14" s="19" t="n"/>
+      <c r="E14" s="3" t="n"/>
+      <c r="F14" s="3" t="n"/>
+      <c r="G14" s="3" t="n"/>
+      <c r="H14" s="14" t="n"/>
+      <c r="I14" s="3" t="n"/>
+      <c r="J14" s="3" t="n"/>
+      <c r="K14" s="3" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="n"/>
-      <c r="B15" s="4" t="n"/>
-      <c r="C15" s="3" t="n"/>
-      <c r="D15" s="3" t="n"/>
-      <c r="E15" s="4" t="n"/>
-      <c r="F15" s="4" t="n"/>
-      <c r="G15" s="4" t="n"/>
-      <c r="H15" s="15" t="n"/>
-      <c r="I15" s="4" t="n"/>
+      <c r="A15" s="3" t="n"/>
+      <c r="B15" s="3" t="n"/>
+      <c r="C15" s="19" t="n"/>
+      <c r="D15" s="19" t="n"/>
+      <c r="E15" s="3" t="n"/>
+      <c r="F15" s="3" t="n"/>
+      <c r="G15" s="3" t="n"/>
+      <c r="H15" s="14" t="n"/>
+      <c r="I15" s="3" t="n"/>
+      <c r="J15" s="3" t="n"/>
+      <c r="K15" s="3" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="n"/>
-      <c r="B16" s="4" t="n"/>
-      <c r="C16" s="3" t="n"/>
-      <c r="D16" s="3" t="n"/>
-      <c r="E16" s="4" t="n"/>
-      <c r="F16" s="4" t="n"/>
-      <c r="G16" s="4" t="n"/>
-      <c r="H16" s="15" t="n"/>
-      <c r="I16" s="4" t="n"/>
+      <c r="A16" s="3" t="n"/>
+      <c r="B16" s="3" t="n"/>
+      <c r="C16" s="19" t="n"/>
+      <c r="D16" s="19" t="n"/>
+      <c r="E16" s="3" t="n"/>
+      <c r="F16" s="3" t="n"/>
+      <c r="G16" s="3" t="n"/>
+      <c r="H16" s="14" t="n"/>
+      <c r="I16" s="3" t="n"/>
+      <c r="J16" s="3" t="n"/>
+      <c r="K16" s="3" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="n"/>
-      <c r="B17" s="4" t="n"/>
-      <c r="C17" s="3" t="n"/>
-      <c r="D17" s="3" t="n"/>
-      <c r="E17" s="4" t="n"/>
-      <c r="F17" s="4" t="n"/>
-      <c r="G17" s="4" t="n"/>
-      <c r="H17" s="15" t="n"/>
-      <c r="I17" s="4" t="n"/>
+      <c r="A17" s="3" t="n"/>
+      <c r="B17" s="3" t="n"/>
+      <c r="C17" s="19" t="n"/>
+      <c r="D17" s="19" t="n"/>
+      <c r="E17" s="3" t="n"/>
+      <c r="F17" s="3" t="n"/>
+      <c r="G17" s="3" t="n"/>
+      <c r="H17" s="14" t="n"/>
+      <c r="I17" s="3" t="n"/>
+      <c r="J17" s="3" t="n"/>
+      <c r="K17" s="3" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="n"/>
-      <c r="B18" s="4" t="n"/>
-      <c r="C18" s="3" t="n"/>
-      <c r="D18" s="3" t="n"/>
-      <c r="E18" s="4" t="n"/>
-      <c r="F18" s="4" t="n"/>
-      <c r="G18" s="4" t="n"/>
-      <c r="H18" s="15" t="n"/>
-      <c r="I18" s="4" t="n"/>
+      <c r="A18" s="3" t="n"/>
+      <c r="B18" s="3" t="n"/>
+      <c r="C18" s="19" t="n"/>
+      <c r="D18" s="19" t="n"/>
+      <c r="E18" s="3" t="n"/>
+      <c r="F18" s="3" t="n"/>
+      <c r="G18" s="3" t="n"/>
+      <c r="H18" s="14" t="n"/>
+      <c r="I18" s="3" t="n"/>
+      <c r="J18" s="3" t="n"/>
+      <c r="K18" s="3" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="n"/>
-      <c r="B19" s="4" t="n"/>
-      <c r="C19" s="3" t="n"/>
-      <c r="D19" s="3" t="n"/>
-      <c r="E19" s="4" t="n"/>
-      <c r="F19" s="4" t="n"/>
-      <c r="G19" s="4" t="n"/>
-      <c r="H19" s="15" t="n"/>
-      <c r="I19" s="4" t="n"/>
+      <c r="A19" s="3" t="n"/>
+      <c r="B19" s="3" t="n"/>
+      <c r="C19" s="19" t="n"/>
+      <c r="D19" s="19" t="n"/>
+      <c r="E19" s="3" t="n"/>
+      <c r="F19" s="3" t="n"/>
+      <c r="G19" s="3" t="n"/>
+      <c r="H19" s="14" t="n"/>
+      <c r="I19" s="3" t="n"/>
+      <c r="J19" s="3" t="n"/>
+      <c r="K19" s="3" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="n"/>
-      <c r="B20" s="4" t="n"/>
-      <c r="C20" s="3" t="n"/>
-      <c r="D20" s="3" t="n"/>
-      <c r="E20" s="4" t="n"/>
-      <c r="F20" s="4" t="n"/>
-      <c r="G20" s="4" t="n"/>
-      <c r="H20" s="15" t="n"/>
-      <c r="I20" s="4" t="n"/>
+      <c r="A20" s="3" t="n"/>
+      <c r="B20" s="3" t="n"/>
+      <c r="C20" s="19" t="n"/>
+      <c r="D20" s="19" t="n"/>
+      <c r="E20" s="3" t="n"/>
+      <c r="F20" s="3" t="n"/>
+      <c r="G20" s="3" t="n"/>
+      <c r="H20" s="14" t="n"/>
+      <c r="I20" s="3" t="n"/>
+      <c r="J20" s="3" t="n"/>
+      <c r="K20" s="3" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="n"/>
-      <c r="B21" s="4" t="n"/>
-      <c r="C21" s="3" t="n"/>
-      <c r="D21" s="3" t="n"/>
-      <c r="E21" s="4" t="n"/>
-      <c r="F21" s="4" t="n"/>
-      <c r="G21" s="4" t="n"/>
-      <c r="H21" s="16" t="n"/>
+      <c r="A21" s="3" t="n"/>
+      <c r="B21" s="3" t="n"/>
+      <c r="C21" s="19" t="n"/>
+      <c r="D21" s="19" t="n"/>
+      <c r="E21" s="3" t="n"/>
+      <c r="F21" s="3" t="n"/>
+      <c r="G21" s="3" t="n"/>
+      <c r="H21" s="14" t="n"/>
+      <c r="I21" s="3" t="n"/>
+      <c r="J21" s="3" t="n"/>
+      <c r="K21" s="3" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="n"/>
-      <c r="B22" s="4" t="n"/>
-      <c r="C22" s="3" t="n"/>
-      <c r="D22" s="3" t="n"/>
-      <c r="E22" s="4" t="n"/>
-      <c r="F22" s="4" t="n"/>
-      <c r="G22" s="14" t="n"/>
-      <c r="H22" s="12" t="n"/>
+      <c r="A22" s="3" t="n"/>
+      <c r="B22" s="3" t="n"/>
+      <c r="C22" s="19" t="n"/>
+      <c r="D22" s="19" t="n"/>
+      <c r="E22" s="3" t="n"/>
+      <c r="F22" s="3" t="n"/>
+      <c r="G22" s="13" t="n"/>
+      <c r="H22" s="14" t="n"/>
+      <c r="I22" s="3" t="n"/>
+      <c r="J22" s="3" t="n"/>
+      <c r="K22" s="3" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="n"/>
-      <c r="B23" s="4" t="n"/>
-      <c r="C23" s="3" t="n"/>
-      <c r="D23" s="3" t="n"/>
-      <c r="E23" s="4" t="n"/>
-      <c r="F23" s="4" t="n"/>
-      <c r="G23" s="4" t="n"/>
-      <c r="H23" s="12" t="n"/>
+      <c r="A23" s="3" t="n"/>
+      <c r="B23" s="3" t="n"/>
+      <c r="C23" s="19" t="n"/>
+      <c r="D23" s="19" t="n"/>
+      <c r="E23" s="3" t="n"/>
+      <c r="F23" s="3" t="n"/>
+      <c r="G23" s="3" t="n"/>
+      <c r="H23" s="14" t="n"/>
+      <c r="I23" s="3" t="n"/>
+      <c r="J23" s="3" t="n"/>
+      <c r="K23" s="3" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="n"/>
-      <c r="B24" s="4" t="n"/>
-      <c r="C24" s="3" t="n"/>
-      <c r="D24" s="3" t="n"/>
-      <c r="E24" s="4" t="n"/>
-      <c r="F24" s="4" t="n"/>
-      <c r="G24" s="4" t="n"/>
-      <c r="H24" s="12" t="n"/>
+      <c r="A24" s="3" t="n"/>
+      <c r="B24" s="3" t="n"/>
+      <c r="C24" s="19" t="n"/>
+      <c r="D24" s="19" t="n"/>
+      <c r="E24" s="3" t="n"/>
+      <c r="F24" s="3" t="n"/>
+      <c r="G24" s="3" t="n"/>
+      <c r="H24" s="14" t="n"/>
+      <c r="I24" s="3" t="n"/>
+      <c r="J24" s="3" t="n"/>
+      <c r="K24" s="3" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="n"/>
-      <c r="B25" s="4" t="n"/>
-      <c r="C25" s="3" t="n"/>
-      <c r="D25" s="3" t="n"/>
-      <c r="E25" s="4" t="n"/>
-      <c r="F25" s="4" t="n"/>
-      <c r="G25" s="4" t="n"/>
-      <c r="H25" s="12" t="n"/>
+      <c r="A25" s="3" t="n"/>
+      <c r="B25" s="3" t="n"/>
+      <c r="C25" s="19" t="n"/>
+      <c r="D25" s="19" t="n"/>
+      <c r="E25" s="3" t="n"/>
+      <c r="F25" s="3" t="n"/>
+      <c r="G25" s="3" t="n"/>
+      <c r="H25" s="14" t="n"/>
+      <c r="I25" s="3" t="n"/>
+      <c r="J25" s="3" t="n"/>
+      <c r="K25" s="3" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="n"/>
-      <c r="B26" s="4" t="n"/>
-      <c r="C26" s="3" t="n"/>
-      <c r="D26" s="3" t="n"/>
-      <c r="E26" s="4" t="n"/>
-      <c r="F26" s="4" t="n"/>
-      <c r="G26" s="4" t="n"/>
-      <c r="H26" s="12" t="n"/>
+      <c r="A26" s="3" t="n"/>
+      <c r="B26" s="3" t="n"/>
+      <c r="C26" s="19" t="n"/>
+      <c r="D26" s="19" t="n"/>
+      <c r="E26" s="3" t="n"/>
+      <c r="F26" s="3" t="n"/>
+      <c r="G26" s="3" t="n"/>
+      <c r="H26" s="14" t="n"/>
+      <c r="I26" s="3" t="n"/>
+      <c r="J26" s="3" t="n"/>
+      <c r="K26" s="3" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="n"/>
-      <c r="B27" s="4" t="n"/>
-      <c r="C27" s="3" t="n"/>
-      <c r="D27" s="3" t="n"/>
-      <c r="E27" s="4" t="n"/>
-      <c r="F27" s="4" t="n"/>
-      <c r="G27" s="4" t="n"/>
-      <c r="H27" s="12" t="n"/>
+      <c r="A27" s="3" t="n"/>
+      <c r="B27" s="3" t="n"/>
+      <c r="C27" s="19" t="n"/>
+      <c r="D27" s="19" t="n"/>
+      <c r="E27" s="3" t="n"/>
+      <c r="F27" s="3" t="n"/>
+      <c r="G27" s="3" t="n"/>
+      <c r="H27" s="14" t="n"/>
+      <c r="I27" s="3" t="n"/>
+      <c r="J27" s="3" t="n"/>
+      <c r="K27" s="3" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="n"/>
-      <c r="B28" s="4" t="n"/>
-      <c r="C28" s="3" t="n"/>
-      <c r="D28" s="3" t="n"/>
-      <c r="E28" s="4" t="n"/>
-      <c r="F28" s="4" t="n"/>
-      <c r="G28" s="4" t="n"/>
-      <c r="H28" s="12" t="n"/>
+      <c r="A28" s="3" t="n"/>
+      <c r="B28" s="3" t="n"/>
+      <c r="C28" s="19" t="n"/>
+      <c r="D28" s="19" t="n"/>
+      <c r="E28" s="3" t="n"/>
+      <c r="F28" s="3" t="n"/>
+      <c r="G28" s="3" t="n"/>
+      <c r="H28" s="14" t="n"/>
+      <c r="I28" s="3" t="n"/>
+      <c r="J28" s="3" t="n"/>
+      <c r="K28" s="3" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="n"/>
-      <c r="B29" s="4" t="n"/>
-      <c r="C29" s="3" t="n"/>
-      <c r="D29" s="3" t="n"/>
-      <c r="E29" s="4" t="n"/>
-      <c r="F29" s="4" t="n"/>
-      <c r="G29" s="4" t="n"/>
-      <c r="H29" s="12" t="n"/>
+      <c r="A29" s="3" t="n"/>
+      <c r="B29" s="3" t="n"/>
+      <c r="C29" s="19" t="n"/>
+      <c r="D29" s="19" t="n"/>
+      <c r="E29" s="3" t="n"/>
+      <c r="F29" s="3" t="n"/>
+      <c r="G29" s="3" t="n"/>
+      <c r="H29" s="14" t="n"/>
+      <c r="I29" s="3" t="n"/>
+      <c r="J29" s="3" t="n"/>
+      <c r="K29" s="3" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="n"/>
-      <c r="B30" s="4" t="n"/>
-      <c r="C30" s="3" t="n"/>
-      <c r="D30" s="3" t="n"/>
-      <c r="E30" s="4" t="n"/>
-      <c r="F30" s="4" t="n"/>
-      <c r="G30" s="4" t="n"/>
-      <c r="H30" s="12" t="n"/>
+      <c r="A30" s="3" t="n"/>
+      <c r="B30" s="3" t="n"/>
+      <c r="C30" s="19" t="n"/>
+      <c r="D30" s="19" t="n"/>
+      <c r="E30" s="3" t="n"/>
+      <c r="F30" s="3" t="n"/>
+      <c r="G30" s="3" t="n"/>
+      <c r="H30" s="11" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="n"/>
-      <c r="B31" s="4" t="n"/>
-      <c r="C31" s="3" t="n"/>
-      <c r="D31" s="3" t="n"/>
-      <c r="E31" s="4" t="n"/>
-      <c r="F31" s="4" t="n"/>
-      <c r="G31" s="4" t="n"/>
-      <c r="H31" s="12" t="n"/>
+      <c r="A31" s="3" t="n"/>
+      <c r="B31" s="3" t="n"/>
+      <c r="C31" s="19" t="n"/>
+      <c r="D31" s="19" t="n"/>
+      <c r="E31" s="3" t="n"/>
+      <c r="F31" s="3" t="n"/>
+      <c r="G31" s="3" t="n"/>
+      <c r="H31" s="11" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="n"/>
-      <c r="B32" s="4" t="n"/>
-      <c r="C32" s="4" t="n"/>
-      <c r="D32" s="4" t="n"/>
-      <c r="E32" s="4" t="n"/>
-      <c r="F32" s="4" t="n"/>
-      <c r="G32" s="4" t="n"/>
+      <c r="A32" s="3" t="n"/>
+      <c r="B32" s="3" t="n"/>
+      <c r="C32" s="3" t="n"/>
+      <c r="D32" s="3" t="n"/>
+      <c r="E32" s="3" t="n"/>
+      <c r="F32" s="3" t="n"/>
+      <c r="G32" s="3" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="n"/>
-      <c r="B33" s="4" t="n"/>
-      <c r="C33" s="4" t="n"/>
-      <c r="D33" s="4" t="n"/>
-      <c r="E33" s="4" t="n"/>
-      <c r="F33" s="4" t="n"/>
-      <c r="G33" s="4" t="n"/>
+      <c r="A33" s="3" t="n"/>
+      <c r="B33" s="3" t="n"/>
+      <c r="C33" s="3" t="n"/>
+      <c r="D33" s="3" t="n"/>
+      <c r="E33" s="3" t="n"/>
+      <c r="F33" s="3" t="n"/>
+      <c r="G33" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -997,81 +1146,81 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="60.42578125" customWidth="1" style="7" min="1" max="1"/>
+    <col width="60.42578125" customWidth="1" style="6" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="29.1" customHeight="1" s="7">
-      <c r="A1" s="10" t="n">
+    <row r="1" ht="29.1" customHeight="1" s="6">
+      <c r="A1" s="9" t="n">
         <v>1192237</v>
       </c>
-      <c r="C1" s="18" t="inlineStr">
+      <c r="C1" s="16" t="inlineStr">
         <is>
           <t>3087 N  Haussen Ct</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">Robert L Jacob </t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Chicago</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F1" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">IL-60618 </t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Cook</t>
         </is>
       </c>
-      <c r="H1" s="15" t="n"/>
-      <c r="I1" s="4" t="n"/>
-    </row>
-    <row r="2" ht="43.5" customHeight="1" s="7">
-      <c r="A2" s="5" t="n">
+      <c r="H1" s="14" t="n"/>
+      <c r="I1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="43.5" customHeight="1" s="6">
+      <c r="A2" s="4" t="n">
         <v>1170191</v>
       </c>
       <c r="B2" s="2" t="n"/>
-      <c r="C2" s="19" t="inlineStr">
+      <c r="C2" s="17" t="inlineStr">
         <is>
           <t>1915 Washington Ave</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="D2" s="19" t="inlineStr">
         <is>
           <t>OBrien Mills</t>
         </is>
       </c>
-      <c r="E2" s="20" t="inlineStr">
+      <c r="E2" s="18" t="inlineStr">
         <is>
           <t>Wilmette</t>
         </is>
       </c>
-      <c r="F2" s="4" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>IL- 60091</t>
         </is>
       </c>
-      <c r="G2" s="4" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>Cook</t>
         </is>
       </c>
-      <c r="H2" s="15" t="n"/>
+      <c r="H2" s="14" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="10" t="n"/>
-      <c r="C3" s="18" t="n"/>
-      <c r="D3" s="3" t="n"/>
-      <c r="E3" s="4" t="n"/>
-      <c r="F3" s="11" t="n"/>
-      <c r="G3" s="4" t="n"/>
-      <c r="H3" s="15" t="n"/>
+      <c r="A3" s="9" t="n"/>
+      <c r="C3" s="16" t="n"/>
+      <c r="D3" s="19" t="n"/>
+      <c r="E3" s="3" t="n"/>
+      <c r="F3" s="10" t="n"/>
+      <c r="G3" s="3" t="n"/>
+      <c r="H3" s="14" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>

</xml_diff>

<commit_message>
NteroSearch exe working 22nd may
</commit_message>
<xml_diff>
--- a/Input/Cook_county.xlsx
+++ b/Input/Cook_county.xlsx
@@ -119,7 +119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -169,9 +169,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -564,8 +561,8 @@
     <col width="19.5703125" customWidth="1" style="2" min="9" max="9"/>
     <col width="24.140625" customWidth="1" style="2" min="10" max="10"/>
     <col width="24.5703125" customWidth="1" style="2" min="11" max="11"/>
-    <col width="8.7109375" customWidth="1" style="2" min="12" max="33"/>
-    <col width="8.7109375" customWidth="1" style="2" min="34" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="12" max="35"/>
+    <col width="8.7109375" customWidth="1" style="2" min="36" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -639,7 +636,7 @@
           <t>67 Indianwood Dr</t>
         </is>
       </c>
-      <c r="D2" s="20" t="inlineStr">
+      <c r="D2" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">NICOLE FISHER </t>
         </is>
@@ -665,11 +662,11 @@
         </is>
       </c>
       <c r="I2" s="3" t="n"/>
-      <c r="J2" s="20" t="n">
-        <v>45068.50023203704</v>
-      </c>
-      <c r="K2" s="20" t="n">
-        <v>45068.52014737268</v>
+      <c r="J2" s="19" t="n">
+        <v>45068.57916152778</v>
+      </c>
+      <c r="K2" s="19" t="n">
+        <v>45068.58425828704</v>
       </c>
     </row>
     <row r="3">
@@ -678,7 +675,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Maximum Retry Error</t>
+          <t>27-10-102-011-0000</t>
         </is>
       </c>
       <c r="C3" s="16" t="inlineStr">
@@ -686,7 +683,7 @@
           <t>9249 145th St</t>
         </is>
       </c>
-      <c r="D3" s="20" t="inlineStr">
+      <c r="D3" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">JONATHAN KITS </t>
         </is>
@@ -712,10 +709,10 @@
         </is>
       </c>
       <c r="I3" s="3" t="n"/>
-      <c r="J3" s="20" t="n">
-        <v>45068.52014791666</v>
-      </c>
-      <c r="K3" s="20" t="n">
+      <c r="J3" s="19" t="n">
+        <v>45068.58425988426</v>
+      </c>
+      <c r="K3" s="19" t="n">
         <v>45065.67318678241</v>
       </c>
     </row>
@@ -723,17 +720,12 @@
       <c r="A4" s="9" t="n">
         <v>1192237</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Maximum Retry Error</t>
-        </is>
-      </c>
       <c r="C4" s="16" t="inlineStr">
         <is>
           <t>3087 N  Haussen Ct</t>
         </is>
       </c>
-      <c r="D4" s="20" t="inlineStr">
+      <c r="D4" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">Robert L Jacob </t>
         </is>
@@ -759,18 +751,18 @@
         </is>
       </c>
       <c r="I4" s="3" t="n"/>
-      <c r="J4" s="20" t="n">
-        <v>45068.5206337037</v>
-      </c>
-      <c r="K4" s="20" t="n">
+      <c r="J4" s="19" t="n">
+        <v>45068.55544650463</v>
+      </c>
+      <c r="K4" s="19" t="n">
         <v>45065.67844310185</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n"/>
       <c r="B5" s="3" t="n"/>
-      <c r="C5" s="20" t="n"/>
-      <c r="D5" s="20" t="n"/>
+      <c r="C5" s="19" t="n"/>
+      <c r="D5" s="19" t="n"/>
       <c r="E5" s="3" t="n"/>
       <c r="F5" s="3" t="n"/>
       <c r="G5" s="18" t="n"/>
@@ -782,8 +774,8 @@
     <row r="6">
       <c r="A6" s="4" t="n"/>
       <c r="B6" s="3" t="n"/>
-      <c r="C6" s="20" t="n"/>
-      <c r="D6" s="20" t="n"/>
+      <c r="C6" s="19" t="n"/>
+      <c r="D6" s="19" t="n"/>
       <c r="E6" s="3" t="n"/>
       <c r="F6" s="3" t="n"/>
       <c r="G6" s="3" t="n"/>
@@ -795,8 +787,8 @@
     <row r="7">
       <c r="A7" s="3" t="n"/>
       <c r="B7" s="3" t="n"/>
-      <c r="C7" s="20" t="n"/>
-      <c r="D7" s="20" t="n"/>
+      <c r="C7" s="19" t="n"/>
+      <c r="D7" s="19" t="n"/>
       <c r="E7" s="3" t="n"/>
       <c r="F7" s="3" t="n"/>
       <c r="G7" s="3" t="n"/>
@@ -808,8 +800,8 @@
     <row r="8">
       <c r="A8" s="3" t="n"/>
       <c r="B8" s="3" t="n"/>
-      <c r="C8" s="20" t="n"/>
-      <c r="D8" s="20" t="n"/>
+      <c r="C8" s="19" t="n"/>
+      <c r="D8" s="19" t="n"/>
       <c r="E8" s="3" t="n"/>
       <c r="F8" s="3" t="n"/>
       <c r="G8" s="3" t="n"/>
@@ -821,8 +813,8 @@
     <row r="9">
       <c r="A9" s="4" t="n"/>
       <c r="B9" s="3" t="n"/>
-      <c r="C9" s="20" t="n"/>
-      <c r="D9" s="20" t="n"/>
+      <c r="C9" s="19" t="n"/>
+      <c r="D9" s="19" t="n"/>
       <c r="E9" s="3" t="n"/>
       <c r="F9" s="3" t="n"/>
       <c r="G9" s="3" t="n"/>
@@ -834,8 +826,8 @@
     <row r="10">
       <c r="A10" s="3" t="n"/>
       <c r="B10" s="3" t="n"/>
-      <c r="C10" s="20" t="n"/>
-      <c r="D10" s="20" t="n"/>
+      <c r="C10" s="19" t="n"/>
+      <c r="D10" s="19" t="n"/>
       <c r="E10" s="3" t="n"/>
       <c r="F10" s="3" t="n"/>
       <c r="G10" s="3" t="n"/>
@@ -847,8 +839,8 @@
     <row r="11">
       <c r="A11" s="3" t="n"/>
       <c r="B11" s="3" t="n"/>
-      <c r="C11" s="20" t="n"/>
-      <c r="D11" s="20" t="n"/>
+      <c r="C11" s="19" t="n"/>
+      <c r="D11" s="19" t="n"/>
       <c r="E11" s="3" t="n"/>
       <c r="F11" s="3" t="n"/>
       <c r="G11" s="3" t="n"/>
@@ -861,7 +853,7 @@
       <c r="A12" s="3" t="n"/>
       <c r="B12" s="3" t="n"/>
       <c r="C12" s="12" t="n"/>
-      <c r="D12" s="20" t="n"/>
+      <c r="D12" s="19" t="n"/>
       <c r="E12" s="3" t="n"/>
       <c r="F12" s="3" t="n"/>
       <c r="G12" s="3" t="n"/>
@@ -874,7 +866,7 @@
       <c r="A13" s="3" t="n"/>
       <c r="B13" s="4" t="n"/>
       <c r="C13" s="12" t="n"/>
-      <c r="D13" s="20" t="n"/>
+      <c r="D13" s="19" t="n"/>
       <c r="E13" s="3" t="n"/>
       <c r="F13" s="3" t="n"/>
       <c r="G13" s="3" t="n"/>
@@ -887,7 +879,7 @@
       <c r="A14" s="3" t="n"/>
       <c r="B14" s="3" t="n"/>
       <c r="C14" s="12" t="n"/>
-      <c r="D14" s="20" t="n"/>
+      <c r="D14" s="19" t="n"/>
       <c r="E14" s="3" t="n"/>
       <c r="F14" s="3" t="n"/>
       <c r="G14" s="3" t="n"/>
@@ -899,8 +891,8 @@
     <row r="15">
       <c r="A15" s="3" t="n"/>
       <c r="B15" s="3" t="n"/>
-      <c r="C15" s="20" t="n"/>
-      <c r="D15" s="20" t="n"/>
+      <c r="C15" s="19" t="n"/>
+      <c r="D15" s="19" t="n"/>
       <c r="E15" s="3" t="n"/>
       <c r="F15" s="3" t="n"/>
       <c r="G15" s="3" t="n"/>
@@ -912,8 +904,8 @@
     <row r="16">
       <c r="A16" s="3" t="n"/>
       <c r="B16" s="3" t="n"/>
-      <c r="C16" s="20" t="n"/>
-      <c r="D16" s="20" t="n"/>
+      <c r="C16" s="19" t="n"/>
+      <c r="D16" s="19" t="n"/>
       <c r="E16" s="3" t="n"/>
       <c r="F16" s="3" t="n"/>
       <c r="G16" s="3" t="n"/>
@@ -925,8 +917,8 @@
     <row r="17">
       <c r="A17" s="3" t="n"/>
       <c r="B17" s="3" t="n"/>
-      <c r="C17" s="20" t="n"/>
-      <c r="D17" s="20" t="n"/>
+      <c r="C17" s="19" t="n"/>
+      <c r="D17" s="19" t="n"/>
       <c r="E17" s="3" t="n"/>
       <c r="F17" s="3" t="n"/>
       <c r="G17" s="3" t="n"/>
@@ -938,8 +930,8 @@
     <row r="18">
       <c r="A18" s="3" t="n"/>
       <c r="B18" s="3" t="n"/>
-      <c r="C18" s="20" t="n"/>
-      <c r="D18" s="20" t="n"/>
+      <c r="C18" s="19" t="n"/>
+      <c r="D18" s="19" t="n"/>
       <c r="E18" s="3" t="n"/>
       <c r="F18" s="3" t="n"/>
       <c r="G18" s="3" t="n"/>
@@ -951,8 +943,8 @@
     <row r="19">
       <c r="A19" s="3" t="n"/>
       <c r="B19" s="3" t="n"/>
-      <c r="C19" s="20" t="n"/>
-      <c r="D19" s="20" t="n"/>
+      <c r="C19" s="19" t="n"/>
+      <c r="D19" s="19" t="n"/>
       <c r="E19" s="3" t="n"/>
       <c r="F19" s="3" t="n"/>
       <c r="G19" s="3" t="n"/>
@@ -964,8 +956,8 @@
     <row r="20">
       <c r="A20" s="3" t="n"/>
       <c r="B20" s="3" t="n"/>
-      <c r="C20" s="20" t="n"/>
-      <c r="D20" s="20" t="n"/>
+      <c r="C20" s="19" t="n"/>
+      <c r="D20" s="19" t="n"/>
       <c r="E20" s="3" t="n"/>
       <c r="F20" s="3" t="n"/>
       <c r="G20" s="3" t="n"/>
@@ -977,8 +969,8 @@
     <row r="21">
       <c r="A21" s="3" t="n"/>
       <c r="B21" s="3" t="n"/>
-      <c r="C21" s="20" t="n"/>
-      <c r="D21" s="20" t="n"/>
+      <c r="C21" s="19" t="n"/>
+      <c r="D21" s="19" t="n"/>
       <c r="E21" s="3" t="n"/>
       <c r="F21" s="3" t="n"/>
       <c r="G21" s="3" t="n"/>
@@ -990,8 +982,8 @@
     <row r="22">
       <c r="A22" s="3" t="n"/>
       <c r="B22" s="3" t="n"/>
-      <c r="C22" s="20" t="n"/>
-      <c r="D22" s="20" t="n"/>
+      <c r="C22" s="19" t="n"/>
+      <c r="D22" s="19" t="n"/>
       <c r="E22" s="3" t="n"/>
       <c r="F22" s="3" t="n"/>
       <c r="G22" s="13" t="n"/>
@@ -1003,8 +995,8 @@
     <row r="23">
       <c r="A23" s="3" t="n"/>
       <c r="B23" s="3" t="n"/>
-      <c r="C23" s="20" t="n"/>
-      <c r="D23" s="20" t="n"/>
+      <c r="C23" s="19" t="n"/>
+      <c r="D23" s="19" t="n"/>
       <c r="E23" s="3" t="n"/>
       <c r="F23" s="3" t="n"/>
       <c r="G23" s="3" t="n"/>
@@ -1016,8 +1008,8 @@
     <row r="24">
       <c r="A24" s="3" t="n"/>
       <c r="B24" s="3" t="n"/>
-      <c r="C24" s="20" t="n"/>
-      <c r="D24" s="20" t="n"/>
+      <c r="C24" s="19" t="n"/>
+      <c r="D24" s="19" t="n"/>
       <c r="E24" s="3" t="n"/>
       <c r="F24" s="3" t="n"/>
       <c r="G24" s="3" t="n"/>
@@ -1029,8 +1021,8 @@
     <row r="25">
       <c r="A25" s="3" t="n"/>
       <c r="B25" s="3" t="n"/>
-      <c r="C25" s="20" t="n"/>
-      <c r="D25" s="20" t="n"/>
+      <c r="C25" s="19" t="n"/>
+      <c r="D25" s="19" t="n"/>
       <c r="E25" s="3" t="n"/>
       <c r="F25" s="3" t="n"/>
       <c r="G25" s="3" t="n"/>
@@ -1042,8 +1034,8 @@
     <row r="26">
       <c r="A26" s="3" t="n"/>
       <c r="B26" s="3" t="n"/>
-      <c r="C26" s="20" t="n"/>
-      <c r="D26" s="20" t="n"/>
+      <c r="C26" s="19" t="n"/>
+      <c r="D26" s="19" t="n"/>
       <c r="E26" s="3" t="n"/>
       <c r="F26" s="3" t="n"/>
       <c r="G26" s="3" t="n"/>
@@ -1055,8 +1047,8 @@
     <row r="27">
       <c r="A27" s="3" t="n"/>
       <c r="B27" s="3" t="n"/>
-      <c r="C27" s="20" t="n"/>
-      <c r="D27" s="20" t="n"/>
+      <c r="C27" s="19" t="n"/>
+      <c r="D27" s="19" t="n"/>
       <c r="E27" s="3" t="n"/>
       <c r="F27" s="3" t="n"/>
       <c r="G27" s="3" t="n"/>
@@ -1068,8 +1060,8 @@
     <row r="28">
       <c r="A28" s="3" t="n"/>
       <c r="B28" s="3" t="n"/>
-      <c r="C28" s="20" t="n"/>
-      <c r="D28" s="20" t="n"/>
+      <c r="C28" s="19" t="n"/>
+      <c r="D28" s="19" t="n"/>
       <c r="E28" s="3" t="n"/>
       <c r="F28" s="3" t="n"/>
       <c r="G28" s="3" t="n"/>
@@ -1081,8 +1073,8 @@
     <row r="29">
       <c r="A29" s="3" t="n"/>
       <c r="B29" s="3" t="n"/>
-      <c r="C29" s="20" t="n"/>
-      <c r="D29" s="20" t="n"/>
+      <c r="C29" s="19" t="n"/>
+      <c r="D29" s="19" t="n"/>
       <c r="E29" s="3" t="n"/>
       <c r="F29" s="3" t="n"/>
       <c r="G29" s="3" t="n"/>
@@ -1094,8 +1086,8 @@
     <row r="30">
       <c r="A30" s="3" t="n"/>
       <c r="B30" s="3" t="n"/>
-      <c r="C30" s="20" t="n"/>
-      <c r="D30" s="20" t="n"/>
+      <c r="C30" s="19" t="n"/>
+      <c r="D30" s="19" t="n"/>
       <c r="E30" s="3" t="n"/>
       <c r="F30" s="3" t="n"/>
       <c r="G30" s="3" t="n"/>
@@ -1104,8 +1096,8 @@
     <row r="31">
       <c r="A31" s="3" t="n"/>
       <c r="B31" s="3" t="n"/>
-      <c r="C31" s="20" t="n"/>
-      <c r="D31" s="20" t="n"/>
+      <c r="C31" s="19" t="n"/>
+      <c r="D31" s="19" t="n"/>
       <c r="E31" s="3" t="n"/>
       <c r="F31" s="3" t="n"/>
       <c r="G31" s="3" t="n"/>
@@ -1161,7 +1153,7 @@
           <t>3087 N  Haussen Ct</t>
         </is>
       </c>
-      <c r="D1" s="20" t="inlineStr">
+      <c r="D1" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">Robert L Jacob </t>
         </is>
@@ -1194,7 +1186,7 @@
           <t>1915 Washington Ave</t>
         </is>
       </c>
-      <c r="D2" s="20" t="inlineStr">
+      <c r="D2" s="19" t="inlineStr">
         <is>
           <t>OBrien Mills</t>
         </is>
@@ -1219,7 +1211,7 @@
     <row r="3">
       <c r="A3" s="9" t="n"/>
       <c r="C3" s="16" t="n"/>
-      <c r="D3" s="20" t="n"/>
+      <c r="D3" s="19" t="n"/>
       <c r="E3" s="3" t="n"/>
       <c r="F3" s="10" t="n"/>
       <c r="G3" s="3" t="n"/>

</xml_diff>

<commit_message>
updated scenario with filewatcher
</commit_message>
<xml_diff>
--- a/Input/Cook_county.xlsx
+++ b/Input/Cook_county.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,9 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="mm:ss.0;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -119,12 +120,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -159,6 +163,9 @@
     <xf numFmtId="45" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="45" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -171,9 +178,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,584 +547,487 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
     <col width="28" customWidth="1" style="2" min="1" max="1"/>
-    <col width="18.85546875" customWidth="1" style="2" min="2" max="2"/>
+    <col width="18.81640625" customWidth="1" style="2" min="2" max="2"/>
     <col width="27" customWidth="1" style="2" min="3" max="3"/>
-    <col width="24.140625" customWidth="1" style="2" min="4" max="4"/>
-    <col width="21.140625" customWidth="1" style="2" min="5" max="5"/>
-    <col width="30.140625" customWidth="1" style="2" min="6" max="6"/>
-    <col width="32.5703125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="33" customWidth="1" style="2" min="8" max="8"/>
-    <col width="19.5703125" customWidth="1" style="2" min="9" max="9"/>
-    <col width="24.140625" customWidth="1" style="2" min="10" max="10"/>
-    <col width="24.5703125" customWidth="1" style="2" min="11" max="11"/>
-    <col width="8.7109375" customWidth="1" style="2" min="12" max="36"/>
-    <col width="8.7109375" customWidth="1" style="2" min="37" max="16384"/>
+    <col width="24.08984375" customWidth="1" style="2" min="4" max="4"/>
+    <col width="21.1796875" customWidth="1" style="2" min="5" max="5"/>
+    <col width="30.1796875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="32.6328125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="14.7265625" customWidth="1" style="2" min="8" max="8"/>
+    <col width="19.6328125" customWidth="1" style="2" min="9" max="9"/>
+    <col width="8.7265625" customWidth="1" style="2" min="10" max="26"/>
+    <col width="8.7265625" customWidth="1" style="2" min="27" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Order No</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>APN</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>Property Address</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="9" t="inlineStr">
         <is>
           <t>NAME</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="8" t="inlineStr">
         <is>
           <t>City</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>State</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="8" t="inlineStr">
         <is>
           <t>County Name</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="H1" s="8" t="inlineStr">
         <is>
           <t>GTD</t>
         </is>
       </c>
-      <c r="I1" s="15" t="inlineStr">
+      <c r="I1" s="17" t="inlineStr">
         <is>
           <t>Second Name</t>
         </is>
       </c>
-      <c r="J1" s="15" t="inlineStr">
-        <is>
-          <t>Start_time</t>
-        </is>
-      </c>
-      <c r="K1" s="15" t="inlineStr">
-        <is>
-          <t>End_time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="9" t="n">
-        <v>1091017</v>
+    </row>
+    <row r="2" ht="11.5" customHeight="1" s="7">
+      <c r="A2" s="10" t="n">
+        <v>1174604</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>27-10-102-011-0000</t>
-        </is>
-      </c>
-      <c r="C2" s="16" t="inlineStr">
-        <is>
-          <t>9249 145th St</t>
-        </is>
-      </c>
-      <c r="D2" s="19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">JONATHAN KITS </t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>Orland Park</t>
-        </is>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
-        <is>
-          <t>IL-60462</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
+          <t>Maximum Retry Error</t>
+        </is>
+      </c>
+      <c r="C2" s="18" t="inlineStr">
+        <is>
+          <t>6735 W Schreiber Ave</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Todd R Strother </t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="F2" s="11" t="inlineStr">
+        <is>
+          <t>IL- 60631</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>Cook</t>
         </is>
       </c>
-      <c r="H2" s="14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Documents Indexed Through: 05-05-2023 </t>
-        </is>
-      </c>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" s="19" t="n">
-        <v>45068.61549111111</v>
-      </c>
-      <c r="K2" s="19" t="n">
-        <v>45065.67318678241</v>
-      </c>
-    </row>
-    <row r="3" ht="11.45" customHeight="1" s="6">
-      <c r="A3" s="9" t="n">
-        <v>1102293</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>29-27-407-037-0000</t>
-        </is>
-      </c>
-      <c r="C3" s="16" t="inlineStr">
-        <is>
-          <t>67 Indianwood Dr</t>
-        </is>
-      </c>
-      <c r="D3" s="19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NICOLE FISHER </t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>Thornton</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>IL- 60476</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="H2" s="15" t="n"/>
+      <c r="I2" s="4" t="n"/>
+      <c r="J2" s="21" t="n">
+        <v>45071.48285611111</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="n">
+        <v>1192237</v>
+      </c>
+      <c r="C3" s="18" t="inlineStr">
+        <is>
+          <t>3087 N  Haussen Ct</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Robert L Jacob </t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="F3" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IL-60618 </t>
+        </is>
+      </c>
+      <c r="G3" s="4" t="inlineStr">
         <is>
           <t>Cook</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Documents Indexed Through: 05-05-2023 </t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="n"/>
-      <c r="J3" s="19" t="n">
-        <v>45068.57916152778</v>
-      </c>
-      <c r="K3" s="19" t="n">
-        <v>45068.58425828704</v>
+      <c r="H3" s="15" t="n"/>
+      <c r="I3" s="4" t="n"/>
+      <c r="J3" s="21" t="n">
+        <v>45071.48331185185</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="n">
-        <v>1192237</v>
-      </c>
-      <c r="C4" s="16" t="inlineStr">
-        <is>
-          <t>3087 N  Haussen Ct</t>
-        </is>
-      </c>
-      <c r="D4" s="19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Robert L Jacob </t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>Chicago</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">IL-60618 </t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="inlineStr">
+      <c r="A4" s="5" t="n">
+        <v>1170191</v>
+      </c>
+      <c r="C4" s="19" t="inlineStr">
+        <is>
+          <t>1915 Washington Ave</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>OBrien Mills</t>
+        </is>
+      </c>
+      <c r="E4" s="20" t="inlineStr">
+        <is>
+          <t>Wilmette</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>IL- 60091</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
         <is>
           <t>Cook</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Documents Indexed Through: 05-05-2023 </t>
-        </is>
-      </c>
-      <c r="I4" s="3" t="n"/>
-      <c r="J4" s="19" t="n">
-        <v>45068.55544650463</v>
-      </c>
-      <c r="K4" s="19" t="n">
-        <v>45065.67844310185</v>
+      <c r="H4" s="15" t="n"/>
+      <c r="I4" s="4" t="n"/>
+      <c r="J4" s="21" t="n">
+        <v>45071.48341737876</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n"/>
-      <c r="B5" s="3" t="n"/>
-      <c r="C5" s="19" t="n"/>
-      <c r="D5" s="19" t="n"/>
-      <c r="E5" s="3" t="n"/>
-      <c r="F5" s="3" t="n"/>
-      <c r="G5" s="18" t="n"/>
-      <c r="H5" s="14" t="n"/>
-      <c r="I5" s="3" t="n"/>
-      <c r="J5" s="3" t="n"/>
-      <c r="K5" s="3" t="n"/>
+      <c r="A5" s="4" t="n"/>
+      <c r="B5" s="4" t="n"/>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+      <c r="E5" s="4" t="n"/>
+      <c r="F5" s="4" t="n"/>
+      <c r="G5" s="4" t="n"/>
+      <c r="H5" s="15" t="n"/>
+      <c r="I5" s="4" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="n"/>
-      <c r="B6" s="3" t="n"/>
-      <c r="C6" s="19" t="n"/>
-      <c r="D6" s="19" t="n"/>
-      <c r="E6" s="3" t="n"/>
-      <c r="F6" s="3" t="n"/>
-      <c r="G6" s="3" t="n"/>
-      <c r="H6" s="14" t="n"/>
-      <c r="I6" s="3" t="n"/>
-      <c r="J6" s="3" t="n"/>
-      <c r="K6" s="3" t="n"/>
+      <c r="A6" s="5" t="n"/>
+      <c r="B6" s="4" t="n"/>
+      <c r="C6" s="3" t="n"/>
+      <c r="D6" s="3" t="n"/>
+      <c r="E6" s="4" t="n"/>
+      <c r="F6" s="4" t="n"/>
+      <c r="G6" s="4" t="n"/>
+      <c r="H6" s="15" t="n"/>
+      <c r="I6" s="4" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="n"/>
-      <c r="B7" s="3" t="n"/>
-      <c r="C7" s="19" t="n"/>
-      <c r="D7" s="19" t="n"/>
-      <c r="E7" s="3" t="n"/>
-      <c r="F7" s="3" t="n"/>
-      <c r="G7" s="3" t="n"/>
-      <c r="H7" s="14" t="n"/>
-      <c r="I7" s="3" t="n"/>
-      <c r="J7" s="3" t="n"/>
-      <c r="K7" s="3" t="n"/>
+      <c r="A7" s="4" t="n"/>
+      <c r="B7" s="4" t="n"/>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+      <c r="E7" s="4" t="n"/>
+      <c r="F7" s="4" t="n"/>
+      <c r="G7" s="4" t="n"/>
+      <c r="H7" s="15" t="n"/>
+      <c r="I7" s="4" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n"/>
-      <c r="B8" s="3" t="n"/>
-      <c r="C8" s="19" t="n"/>
-      <c r="D8" s="19" t="n"/>
-      <c r="E8" s="3" t="n"/>
-      <c r="F8" s="3" t="n"/>
-      <c r="G8" s="3" t="n"/>
-      <c r="H8" s="14" t="n"/>
-      <c r="I8" s="3" t="n"/>
-      <c r="J8" s="3" t="n"/>
-      <c r="K8" s="3" t="n"/>
+      <c r="A8" s="4" t="n"/>
+      <c r="B8" s="4" t="n"/>
+      <c r="C8" s="3" t="n"/>
+      <c r="D8" s="3" t="n"/>
+      <c r="E8" s="4" t="n"/>
+      <c r="F8" s="4" t="n"/>
+      <c r="G8" s="4" t="n"/>
+      <c r="H8" s="15" t="n"/>
+      <c r="I8" s="4" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="n"/>
-      <c r="B9" s="3" t="n"/>
-      <c r="C9" s="19" t="n"/>
-      <c r="D9" s="19" t="n"/>
-      <c r="E9" s="3" t="n"/>
-      <c r="F9" s="3" t="n"/>
-      <c r="G9" s="3" t="n"/>
-      <c r="H9" s="14" t="n"/>
-      <c r="I9" s="3" t="n"/>
-      <c r="J9" s="3" t="n"/>
-      <c r="K9" s="3" t="n"/>
+      <c r="A9" s="5" t="n"/>
+      <c r="B9" s="4" t="n"/>
+      <c r="C9" s="3" t="n"/>
+      <c r="D9" s="3" t="n"/>
+      <c r="E9" s="4" t="n"/>
+      <c r="F9" s="4" t="n"/>
+      <c r="G9" s="4" t="n"/>
+      <c r="H9" s="15" t="n"/>
+      <c r="I9" s="4" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="n"/>
-      <c r="B10" s="3" t="n"/>
-      <c r="C10" s="19" t="n"/>
-      <c r="D10" s="19" t="n"/>
-      <c r="E10" s="3" t="n"/>
-      <c r="F10" s="3" t="n"/>
-      <c r="G10" s="3" t="n"/>
-      <c r="H10" s="14" t="n"/>
-      <c r="I10" s="3" t="n"/>
-      <c r="J10" s="3" t="n"/>
-      <c r="K10" s="3" t="n"/>
+      <c r="A10" s="4" t="n"/>
+      <c r="B10" s="4" t="n"/>
+      <c r="C10" s="3" t="n"/>
+      <c r="D10" s="3" t="n"/>
+      <c r="E10" s="4" t="n"/>
+      <c r="F10" s="4" t="n"/>
+      <c r="G10" s="4" t="n"/>
+      <c r="H10" s="15" t="n"/>
+      <c r="I10" s="4" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="n"/>
-      <c r="B11" s="3" t="n"/>
-      <c r="C11" s="19" t="n"/>
-      <c r="D11" s="19" t="n"/>
-      <c r="E11" s="3" t="n"/>
-      <c r="F11" s="3" t="n"/>
-      <c r="G11" s="3" t="n"/>
-      <c r="H11" s="14" t="n"/>
-      <c r="I11" s="3" t="n"/>
-      <c r="J11" s="3" t="n"/>
-      <c r="K11" s="3" t="n"/>
+      <c r="A11" s="4" t="n"/>
+      <c r="B11" s="4" t="n"/>
+      <c r="C11" s="3" t="n"/>
+      <c r="D11" s="3" t="n"/>
+      <c r="E11" s="4" t="n"/>
+      <c r="F11" s="4" t="n"/>
+      <c r="G11" s="4" t="n"/>
+      <c r="H11" s="15" t="n"/>
+      <c r="I11" s="4" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="n"/>
-      <c r="B12" s="3" t="n"/>
-      <c r="C12" s="12" t="n"/>
-      <c r="D12" s="19" t="n"/>
-      <c r="E12" s="3" t="n"/>
-      <c r="F12" s="3" t="n"/>
-      <c r="G12" s="3" t="n"/>
-      <c r="H12" s="14" t="n"/>
-      <c r="I12" s="3" t="n"/>
-      <c r="J12" s="3" t="n"/>
-      <c r="K12" s="3" t="n"/>
+      <c r="A12" s="4" t="n"/>
+      <c r="B12" s="4" t="n"/>
+      <c r="C12" s="13" t="n"/>
+      <c r="D12" s="3" t="n"/>
+      <c r="E12" s="4" t="n"/>
+      <c r="F12" s="4" t="n"/>
+      <c r="G12" s="4" t="n"/>
+      <c r="H12" s="15" t="n"/>
+      <c r="I12" s="4" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="n"/>
-      <c r="B13" s="4" t="n"/>
-      <c r="C13" s="12" t="n"/>
-      <c r="D13" s="19" t="n"/>
-      <c r="E13" s="3" t="n"/>
-      <c r="F13" s="3" t="n"/>
-      <c r="G13" s="3" t="n"/>
-      <c r="H13" s="14" t="n"/>
-      <c r="I13" s="3" t="n"/>
-      <c r="J13" s="3" t="n"/>
-      <c r="K13" s="3" t="n"/>
+      <c r="A13" s="4" t="n"/>
+      <c r="B13" s="5" t="n"/>
+      <c r="C13" s="13" t="n"/>
+      <c r="D13" s="3" t="n"/>
+      <c r="E13" s="4" t="n"/>
+      <c r="F13" s="4" t="n"/>
+      <c r="G13" s="4" t="n"/>
+      <c r="H13" s="15" t="n"/>
+      <c r="I13" s="4" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="n"/>
-      <c r="B14" s="3" t="n"/>
-      <c r="C14" s="12" t="n"/>
-      <c r="D14" s="19" t="n"/>
-      <c r="E14" s="3" t="n"/>
-      <c r="F14" s="3" t="n"/>
-      <c r="G14" s="3" t="n"/>
-      <c r="H14" s="14" t="n"/>
-      <c r="I14" s="3" t="n"/>
-      <c r="J14" s="3" t="n"/>
-      <c r="K14" s="3" t="n"/>
+      <c r="A14" s="4" t="n"/>
+      <c r="B14" s="4" t="n"/>
+      <c r="C14" s="13" t="n"/>
+      <c r="D14" s="3" t="n"/>
+      <c r="E14" s="4" t="n"/>
+      <c r="F14" s="4" t="n"/>
+      <c r="G14" s="4" t="n"/>
+      <c r="H14" s="15" t="n"/>
+      <c r="I14" s="4" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="n"/>
-      <c r="B15" s="3" t="n"/>
-      <c r="C15" s="19" t="n"/>
-      <c r="D15" s="19" t="n"/>
-      <c r="E15" s="3" t="n"/>
-      <c r="F15" s="3" t="n"/>
-      <c r="G15" s="3" t="n"/>
-      <c r="H15" s="14" t="n"/>
-      <c r="I15" s="3" t="n"/>
-      <c r="J15" s="3" t="n"/>
-      <c r="K15" s="3" t="n"/>
+      <c r="A15" s="4" t="n"/>
+      <c r="B15" s="4" t="n"/>
+      <c r="C15" s="3" t="n"/>
+      <c r="D15" s="3" t="n"/>
+      <c r="E15" s="4" t="n"/>
+      <c r="F15" s="4" t="n"/>
+      <c r="G15" s="4" t="n"/>
+      <c r="H15" s="15" t="n"/>
+      <c r="I15" s="4" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="n"/>
-      <c r="B16" s="3" t="n"/>
-      <c r="C16" s="19" t="n"/>
-      <c r="D16" s="19" t="n"/>
-      <c r="E16" s="3" t="n"/>
-      <c r="F16" s="3" t="n"/>
-      <c r="G16" s="3" t="n"/>
-      <c r="H16" s="14" t="n"/>
-      <c r="I16" s="3" t="n"/>
-      <c r="J16" s="3" t="n"/>
-      <c r="K16" s="3" t="n"/>
+      <c r="A16" s="4" t="n"/>
+      <c r="B16" s="4" t="n"/>
+      <c r="C16" s="3" t="n"/>
+      <c r="D16" s="3" t="n"/>
+      <c r="E16" s="4" t="n"/>
+      <c r="F16" s="4" t="n"/>
+      <c r="G16" s="4" t="n"/>
+      <c r="H16" s="15" t="n"/>
+      <c r="I16" s="4" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="n"/>
-      <c r="B17" s="3" t="n"/>
-      <c r="C17" s="19" t="n"/>
-      <c r="D17" s="19" t="n"/>
-      <c r="E17" s="3" t="n"/>
-      <c r="F17" s="3" t="n"/>
-      <c r="G17" s="3" t="n"/>
-      <c r="H17" s="14" t="n"/>
-      <c r="I17" s="3" t="n"/>
-      <c r="J17" s="3" t="n"/>
-      <c r="K17" s="3" t="n"/>
+      <c r="A17" s="4" t="n"/>
+      <c r="B17" s="4" t="n"/>
+      <c r="C17" s="3" t="n"/>
+      <c r="D17" s="3" t="n"/>
+      <c r="E17" s="4" t="n"/>
+      <c r="F17" s="4" t="n"/>
+      <c r="G17" s="4" t="n"/>
+      <c r="H17" s="15" t="n"/>
+      <c r="I17" s="4" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="n"/>
-      <c r="B18" s="3" t="n"/>
-      <c r="C18" s="19" t="n"/>
-      <c r="D18" s="19" t="n"/>
-      <c r="E18" s="3" t="n"/>
-      <c r="F18" s="3" t="n"/>
-      <c r="G18" s="3" t="n"/>
-      <c r="H18" s="14" t="n"/>
-      <c r="I18" s="3" t="n"/>
-      <c r="J18" s="3" t="n"/>
-      <c r="K18" s="3" t="n"/>
+      <c r="A18" s="4" t="n"/>
+      <c r="B18" s="4" t="n"/>
+      <c r="C18" s="3" t="n"/>
+      <c r="D18" s="3" t="n"/>
+      <c r="E18" s="4" t="n"/>
+      <c r="F18" s="4" t="n"/>
+      <c r="G18" s="4" t="n"/>
+      <c r="H18" s="15" t="n"/>
+      <c r="I18" s="4" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="n"/>
-      <c r="B19" s="3" t="n"/>
-      <c r="C19" s="19" t="n"/>
-      <c r="D19" s="19" t="n"/>
-      <c r="E19" s="3" t="n"/>
-      <c r="F19" s="3" t="n"/>
-      <c r="G19" s="3" t="n"/>
-      <c r="H19" s="14" t="n"/>
-      <c r="I19" s="3" t="n"/>
-      <c r="J19" s="3" t="n"/>
-      <c r="K19" s="3" t="n"/>
+      <c r="A19" s="4" t="n"/>
+      <c r="B19" s="4" t="n"/>
+      <c r="C19" s="3" t="n"/>
+      <c r="D19" s="3" t="n"/>
+      <c r="E19" s="4" t="n"/>
+      <c r="F19" s="4" t="n"/>
+      <c r="G19" s="4" t="n"/>
+      <c r="H19" s="15" t="n"/>
+      <c r="I19" s="4" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="n"/>
-      <c r="B20" s="3" t="n"/>
-      <c r="C20" s="19" t="n"/>
-      <c r="D20" s="19" t="n"/>
-      <c r="E20" s="3" t="n"/>
-      <c r="F20" s="3" t="n"/>
-      <c r="G20" s="3" t="n"/>
-      <c r="H20" s="14" t="n"/>
-      <c r="I20" s="3" t="n"/>
-      <c r="J20" s="3" t="n"/>
-      <c r="K20" s="3" t="n"/>
+      <c r="A20" s="4" t="n"/>
+      <c r="B20" s="4" t="n"/>
+      <c r="C20" s="3" t="n"/>
+      <c r="D20" s="3" t="n"/>
+      <c r="E20" s="4" t="n"/>
+      <c r="F20" s="4" t="n"/>
+      <c r="G20" s="4" t="n"/>
+      <c r="H20" s="15" t="n"/>
+      <c r="I20" s="4" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="n"/>
-      <c r="B21" s="3" t="n"/>
-      <c r="C21" s="19" t="n"/>
-      <c r="D21" s="19" t="n"/>
-      <c r="E21" s="3" t="n"/>
-      <c r="F21" s="3" t="n"/>
-      <c r="G21" s="3" t="n"/>
-      <c r="H21" s="14" t="n"/>
-      <c r="I21" s="3" t="n"/>
-      <c r="J21" s="3" t="n"/>
-      <c r="K21" s="3" t="n"/>
+      <c r="A21" s="4" t="n"/>
+      <c r="B21" s="4" t="n"/>
+      <c r="C21" s="3" t="n"/>
+      <c r="D21" s="3" t="n"/>
+      <c r="E21" s="4" t="n"/>
+      <c r="F21" s="4" t="n"/>
+      <c r="G21" s="4" t="n"/>
+      <c r="H21" s="16" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="n"/>
-      <c r="B22" s="3" t="n"/>
-      <c r="C22" s="19" t="n"/>
-      <c r="D22" s="19" t="n"/>
-      <c r="E22" s="3" t="n"/>
-      <c r="F22" s="3" t="n"/>
-      <c r="G22" s="13" t="n"/>
-      <c r="H22" s="14" t="n"/>
-      <c r="I22" s="3" t="n"/>
-      <c r="J22" s="3" t="n"/>
-      <c r="K22" s="3" t="n"/>
+      <c r="A22" s="4" t="n"/>
+      <c r="B22" s="4" t="n"/>
+      <c r="C22" s="3" t="n"/>
+      <c r="D22" s="3" t="n"/>
+      <c r="E22" s="4" t="n"/>
+      <c r="F22" s="4" t="n"/>
+      <c r="G22" s="14" t="n"/>
+      <c r="H22" s="12" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="n"/>
-      <c r="B23" s="3" t="n"/>
-      <c r="C23" s="19" t="n"/>
-      <c r="D23" s="19" t="n"/>
-      <c r="E23" s="3" t="n"/>
-      <c r="F23" s="3" t="n"/>
-      <c r="G23" s="3" t="n"/>
-      <c r="H23" s="14" t="n"/>
-      <c r="I23" s="3" t="n"/>
-      <c r="J23" s="3" t="n"/>
-      <c r="K23" s="3" t="n"/>
+      <c r="A23" s="4" t="n"/>
+      <c r="B23" s="4" t="n"/>
+      <c r="C23" s="3" t="n"/>
+      <c r="D23" s="3" t="n"/>
+      <c r="E23" s="4" t="n"/>
+      <c r="F23" s="4" t="n"/>
+      <c r="G23" s="4" t="n"/>
+      <c r="H23" s="12" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="n"/>
-      <c r="B24" s="3" t="n"/>
-      <c r="C24" s="19" t="n"/>
-      <c r="D24" s="19" t="n"/>
-      <c r="E24" s="3" t="n"/>
-      <c r="F24" s="3" t="n"/>
-      <c r="G24" s="3" t="n"/>
-      <c r="H24" s="14" t="n"/>
-      <c r="I24" s="3" t="n"/>
-      <c r="J24" s="3" t="n"/>
-      <c r="K24" s="3" t="n"/>
+      <c r="A24" s="4" t="n"/>
+      <c r="B24" s="4" t="n"/>
+      <c r="C24" s="3" t="n"/>
+      <c r="D24" s="3" t="n"/>
+      <c r="E24" s="4" t="n"/>
+      <c r="F24" s="4" t="n"/>
+      <c r="G24" s="4" t="n"/>
+      <c r="H24" s="12" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="n"/>
-      <c r="B25" s="3" t="n"/>
-      <c r="C25" s="19" t="n"/>
-      <c r="D25" s="19" t="n"/>
-      <c r="E25" s="3" t="n"/>
-      <c r="F25" s="3" t="n"/>
-      <c r="G25" s="3" t="n"/>
-      <c r="H25" s="14" t="n"/>
-      <c r="I25" s="3" t="n"/>
-      <c r="J25" s="3" t="n"/>
-      <c r="K25" s="3" t="n"/>
+      <c r="A25" s="4" t="n"/>
+      <c r="B25" s="4" t="n"/>
+      <c r="C25" s="3" t="n"/>
+      <c r="D25" s="3" t="n"/>
+      <c r="E25" s="4" t="n"/>
+      <c r="F25" s="4" t="n"/>
+      <c r="G25" s="4" t="n"/>
+      <c r="H25" s="12" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="3" t="n"/>
-      <c r="B26" s="3" t="n"/>
-      <c r="C26" s="19" t="n"/>
-      <c r="D26" s="19" t="n"/>
-      <c r="E26" s="3" t="n"/>
-      <c r="F26" s="3" t="n"/>
-      <c r="G26" s="3" t="n"/>
-      <c r="H26" s="14" t="n"/>
-      <c r="I26" s="3" t="n"/>
-      <c r="J26" s="3" t="n"/>
-      <c r="K26" s="3" t="n"/>
+      <c r="A26" s="4" t="n"/>
+      <c r="B26" s="4" t="n"/>
+      <c r="C26" s="3" t="n"/>
+      <c r="D26" s="3" t="n"/>
+      <c r="E26" s="4" t="n"/>
+      <c r="F26" s="4" t="n"/>
+      <c r="G26" s="4" t="n"/>
+      <c r="H26" s="12" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="n"/>
-      <c r="B27" s="3" t="n"/>
-      <c r="C27" s="19" t="n"/>
-      <c r="D27" s="19" t="n"/>
-      <c r="E27" s="3" t="n"/>
-      <c r="F27" s="3" t="n"/>
-      <c r="G27" s="3" t="n"/>
-      <c r="H27" s="14" t="n"/>
-      <c r="I27" s="3" t="n"/>
-      <c r="J27" s="3" t="n"/>
-      <c r="K27" s="3" t="n"/>
+      <c r="A27" s="4" t="n"/>
+      <c r="B27" s="4" t="n"/>
+      <c r="C27" s="3" t="n"/>
+      <c r="D27" s="3" t="n"/>
+      <c r="E27" s="4" t="n"/>
+      <c r="F27" s="4" t="n"/>
+      <c r="G27" s="4" t="n"/>
+      <c r="H27" s="12" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="n"/>
-      <c r="B28" s="3" t="n"/>
-      <c r="C28" s="19" t="n"/>
-      <c r="D28" s="19" t="n"/>
-      <c r="E28" s="3" t="n"/>
-      <c r="F28" s="3" t="n"/>
-      <c r="G28" s="3" t="n"/>
-      <c r="H28" s="14" t="n"/>
-      <c r="I28" s="3" t="n"/>
-      <c r="J28" s="3" t="n"/>
-      <c r="K28" s="3" t="n"/>
+      <c r="A28" s="4" t="n"/>
+      <c r="B28" s="4" t="n"/>
+      <c r="C28" s="3" t="n"/>
+      <c r="D28" s="3" t="n"/>
+      <c r="E28" s="4" t="n"/>
+      <c r="F28" s="4" t="n"/>
+      <c r="G28" s="4" t="n"/>
+      <c r="H28" s="12" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="n"/>
-      <c r="B29" s="3" t="n"/>
-      <c r="C29" s="19" t="n"/>
-      <c r="D29" s="19" t="n"/>
-      <c r="E29" s="3" t="n"/>
-      <c r="F29" s="3" t="n"/>
-      <c r="G29" s="3" t="n"/>
-      <c r="H29" s="14" t="n"/>
-      <c r="I29" s="3" t="n"/>
-      <c r="J29" s="3" t="n"/>
-      <c r="K29" s="3" t="n"/>
+      <c r="A29" s="4" t="n"/>
+      <c r="B29" s="4" t="n"/>
+      <c r="C29" s="3" t="n"/>
+      <c r="D29" s="3" t="n"/>
+      <c r="E29" s="4" t="n"/>
+      <c r="F29" s="4" t="n"/>
+      <c r="G29" s="4" t="n"/>
+      <c r="H29" s="12" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="3" t="n"/>
-      <c r="B30" s="3" t="n"/>
-      <c r="C30" s="19" t="n"/>
-      <c r="D30" s="19" t="n"/>
-      <c r="E30" s="3" t="n"/>
-      <c r="F30" s="3" t="n"/>
-      <c r="G30" s="3" t="n"/>
-      <c r="H30" s="11" t="n"/>
+      <c r="A30" s="4" t="n"/>
+      <c r="B30" s="4" t="n"/>
+      <c r="C30" s="3" t="n"/>
+      <c r="D30" s="3" t="n"/>
+      <c r="E30" s="4" t="n"/>
+      <c r="F30" s="4" t="n"/>
+      <c r="G30" s="4" t="n"/>
+      <c r="H30" s="12" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="n"/>
-      <c r="B31" s="3" t="n"/>
-      <c r="C31" s="19" t="n"/>
-      <c r="D31" s="19" t="n"/>
-      <c r="E31" s="3" t="n"/>
-      <c r="F31" s="3" t="n"/>
-      <c r="G31" s="3" t="n"/>
-      <c r="H31" s="11" t="n"/>
+      <c r="A31" s="4" t="n"/>
+      <c r="B31" s="4" t="n"/>
+      <c r="C31" s="3" t="n"/>
+      <c r="D31" s="3" t="n"/>
+      <c r="E31" s="4" t="n"/>
+      <c r="F31" s="4" t="n"/>
+      <c r="G31" s="4" t="n"/>
+      <c r="H31" s="12" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="n"/>
-      <c r="B32" s="3" t="n"/>
-      <c r="C32" s="3" t="n"/>
-      <c r="D32" s="3" t="n"/>
-      <c r="E32" s="3" t="n"/>
-      <c r="F32" s="3" t="n"/>
-      <c r="G32" s="3" t="n"/>
+      <c r="A32" s="4" t="n"/>
+      <c r="B32" s="4" t="n"/>
+      <c r="C32" s="4" t="n"/>
+      <c r="D32" s="4" t="n"/>
+      <c r="E32" s="4" t="n"/>
+      <c r="F32" s="4" t="n"/>
+      <c r="G32" s="4" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="n"/>
-      <c r="B33" s="3" t="n"/>
-      <c r="C33" s="3" t="n"/>
-      <c r="D33" s="3" t="n"/>
-      <c r="E33" s="3" t="n"/>
-      <c r="F33" s="3" t="n"/>
-      <c r="G33" s="3" t="n"/>
+      <c r="A33" s="4" t="n"/>
+      <c r="B33" s="4" t="n"/>
+      <c r="C33" s="4" t="n"/>
+      <c r="D33" s="4" t="n"/>
+      <c r="E33" s="4" t="n"/>
+      <c r="F33" s="4" t="n"/>
+      <c r="G33" s="4" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1139,83 +1047,83 @@
       <selection activeCell="A1" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="60.42578125" customWidth="1" style="6" min="1" max="1"/>
+    <col width="60.36328125" customWidth="1" style="7" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="29.1" customHeight="1" s="6">
-      <c r="A1" s="9" t="n">
+    <row r="1" ht="29" customHeight="1" s="7">
+      <c r="A1" s="10" t="n">
         <v>1192237</v>
       </c>
-      <c r="C1" s="16" t="inlineStr">
+      <c r="C1" s="18" t="inlineStr">
         <is>
           <t>3087 N  Haussen Ct</t>
         </is>
       </c>
-      <c r="D1" s="19" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">Robert L Jacob </t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>Chicago</t>
         </is>
       </c>
-      <c r="F1" s="10" t="inlineStr">
+      <c r="F1" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">IL-60618 </t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Cook</t>
         </is>
       </c>
-      <c r="H1" s="14" t="n"/>
-      <c r="I1" s="3" t="n"/>
-    </row>
-    <row r="2" ht="43.5" customHeight="1" s="6">
-      <c r="A2" s="4" t="n">
+      <c r="H1" s="15" t="n"/>
+      <c r="I1" s="4" t="n"/>
+    </row>
+    <row r="2" ht="43.5" customHeight="1" s="7">
+      <c r="A2" s="5" t="n">
         <v>1170191</v>
       </c>
       <c r="B2" s="2" t="n"/>
-      <c r="C2" s="17" t="inlineStr">
+      <c r="C2" s="19" t="inlineStr">
         <is>
           <t>1915 Washington Ave</t>
         </is>
       </c>
-      <c r="D2" s="19" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>OBrien Mills</t>
         </is>
       </c>
-      <c r="E2" s="18" t="inlineStr">
+      <c r="E2" s="20" t="inlineStr">
         <is>
           <t>Wilmette</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>IL- 60091</t>
         </is>
       </c>
-      <c r="G2" s="3" t="inlineStr">
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>Cook</t>
         </is>
       </c>
-      <c r="H2" s="14" t="n"/>
+      <c r="H2" s="15" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="n"/>
-      <c r="C3" s="16" t="n"/>
-      <c r="D3" s="19" t="n"/>
-      <c r="E3" s="3" t="n"/>
-      <c r="F3" s="10" t="n"/>
-      <c r="G3" s="3" t="n"/>
-      <c r="H3" s="14" t="n"/>
+      <c r="A3" s="10" t="n"/>
+      <c r="C3" s="18" t="n"/>
+      <c r="D3" s="3" t="n"/>
+      <c r="E3" s="4" t="n"/>
+      <c r="F3" s="11" t="n"/>
+      <c r="G3" s="4" t="n"/>
+      <c r="H3" s="15" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>

</xml_diff>